<commit_message>
Clean up and Week 3 Submission
-cleaned up week 2 submissions
-commit for week 3 knapsack code
</commit_message>
<xml_diff>
--- a/Week_1/Book1.xlsx
+++ b/Week_1/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0400b1dcfee898cb/Documents/OSU/CS 325/CS325/Week_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="8_{EC1B6870-28A3-453E-A1D0-940CD8FA5C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81A19F0B-6F41-466C-B666-7C9625E4612E}"/>
+  <xr:revisionPtr revIDLastSave="184" documentId="8_{EC1B6870-28A3-453E-A1D0-940CD8FA5C49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C088AE03-F770-41C0-8343-1A66C06ECDED}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{139A86C7-CA04-46DA-95BF-041C89199F04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{139A86C7-CA04-46DA-95BF-041C89199F04}"/>
   </bookViews>
   <sheets>
     <sheet name="mergeTime" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,14 +90,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -837,6 +857,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1333474399"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2803,13 +2824,13 @@
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2820,7 +2841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -2832,7 +2853,7 @@
         <v>3.6666413929882576E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10000</v>
       </c>
@@ -2844,7 +2865,7 @@
         <v>0.62566154104341376</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15000</v>
       </c>
@@ -2856,7 +2877,7 @@
         <v>0.98025671236261602</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20000</v>
       </c>
@@ -2868,7 +2889,7 @@
         <v>1.2259816716255432</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>30000</v>
       </c>
@@ -2880,7 +2901,7 @@
         <v>1.5799005418494976</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40000</v>
       </c>
@@ -2892,7 +2913,7 @@
         <v>1.8354357349758312</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50000</v>
       </c>
@@ -2904,7 +2925,7 @@
         <v>2.0351075810575572</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2915,7 +2936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -2927,7 +2948,7 @@
         <v>3.6666413929882576E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10000</v>
       </c>
@@ -2939,7 +2960,7 @@
         <v>0.62566154104341376</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15000</v>
       </c>
@@ -2951,7 +2972,7 @@
         <v>0.98025671236261602</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20000</v>
       </c>
@@ -2963,7 +2984,7 @@
         <v>1.2259816716255432</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>30000</v>
       </c>
@@ -2975,7 +2996,7 @@
         <v>1.5799005418494976</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40000</v>
       </c>
@@ -2987,7 +3008,7 @@
         <v>1.8354357349758312</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50000</v>
       </c>
@@ -3014,12 +3035,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3027,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -3035,7 +3056,7 @@
         <v>1.0880939960479701</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10000</v>
       </c>
@@ -3043,7 +3064,7 @@
         <v>4.2233934402465803</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15000</v>
       </c>
@@ -3051,7 +3072,7 @@
         <v>9.5555725097656197</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20000</v>
       </c>
@@ -3059,7 +3080,7 @@
         <v>16.8260304927825</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>30000</v>
       </c>
@@ -3067,7 +3088,7 @@
         <v>38.010233879089299</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40000</v>
       </c>
@@ -3075,7 +3096,7 @@
         <v>68.459817171096802</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50000</v>
       </c>
@@ -3093,96 +3114,99 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>100</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0.1031994</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>200</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0.30119400000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>300</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0.92779610000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>400</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2.7087297000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>500</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>8.2646514999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>600</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>8.2296928999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>700</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>8.2791132899999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>800</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>24.702387332000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>900</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>24.796847105000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>1000</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>25.110543966289999</v>
       </c>
     </row>

</xml_diff>